<commit_message>
modify TST936 to run smoothly
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST1353_UninstallationProcess.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST1353_UninstallationProcess.xlsx
@@ -3640,7 +3640,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>C:\\Nform_4.8.1_ET\\SE\\Nform_4.8.1_ET_Setup.exe</t>
+    <t>C:\\Nform_4.8.1\\SE\\Nform_4.8.1_Setup.exe</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -4571,7 +4571,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>